<commit_message>
ajout google search console
</commit_message>
<xml_diff>
--- a/P4_01_analyse.xlsx
+++ b/P4_01_analyse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Formation OC\P4_serra_jahan\Starting_website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Formation OC\P4_serra_jahan\jahanSerra_4_03032021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE39C259-02AF-4CD2-A3DC-BC5AC0CF1D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB86EBFC-A571-41DD-9021-6D45987F4427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2580" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30090" yWindow="3120" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Ajout image redim + correctif seo + correctif accessibilité+sitemap
</commit_message>
<xml_diff>
--- a/P4_01_analyse.xlsx
+++ b/P4_01_analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Formation OC\P4_serra_jahan\jahanSerra_4_03032021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB86EBFC-A571-41DD-9021-6D45987F4427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23286C5-F661-45AB-993D-1CC0128BE92C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30090" yWindow="3120" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>Catégorie</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Adopter un titre de page en rapport avec le contenu</t>
   </si>
   <si>
-    <t>Accessiblité et SEO</t>
-  </si>
-  <si>
     <t>balise html lang= Default</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>mettre fr ici</t>
   </si>
   <si>
-    <t>Changer le titre par un plus cohérent 65 caractères max</t>
-  </si>
-  <si>
     <t>https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t>
   </si>
   <si>
@@ -159,9 +153,6 @@
     <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6940878-decouvrez-les-exigences-en-matiere-daccessibilite</t>
   </si>
   <si>
-    <t>Accessiblité</t>
-  </si>
-  <si>
     <t>taille des images trop grande</t>
   </si>
   <si>
@@ -172,6 +163,42 @@
   </si>
   <si>
     <t>redimensionner les grandes images voir compresser dans la mesure du possible pour gagner au temps de chargement de la page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer le titre par un plus cohérent 65 caractères max </t>
+  </si>
+  <si>
+    <t>balise keyword cachées</t>
+  </si>
+  <si>
+    <t>des balises keyword sont dans le code cela entraine des doublons et une sur utilisation de mots clefs</t>
+  </si>
+  <si>
+    <t>utiliser une fois la balise dans le head</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo</t>
+  </si>
+  <si>
+    <t>Ajouter la balise dans le head et supprimer les autres dans le body</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Accessibilité et SEO</t>
+  </si>
+  <si>
+    <t>Pas d'encre de retour haut de page</t>
+  </si>
+  <si>
+    <t>absence d'encrage</t>
+  </si>
+  <si>
+    <t>Utiliser une encre de retour en haut de page pour l'Accessibilité</t>
+  </si>
+  <si>
+    <t>création de l'id et de la balise de retour en haut de page</t>
   </si>
 </sst>
 </file>
@@ -212,7 +239,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +250,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -246,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,6 +288,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -474,7 +508,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -538,31 +572,31 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
+      <c r="E2" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -570,39 +604,39 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -610,19 +644,19 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -630,19 +664,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -650,39 +684,39 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -690,26 +724,60 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="4"/>
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="4"/>
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E13" s="4"/>
@@ -1716,6 +1784,8 @@
     <hyperlink ref="F8" r:id="rId7" xr:uid="{A8B1B70C-FB45-425E-9C47-7E3200797EF1}"/>
     <hyperlink ref="F9" r:id="rId8" xr:uid="{53DA0DAE-D976-4707-9E4A-C51EFA62A73C}"/>
     <hyperlink ref="F10" r:id="rId9" xr:uid="{2975BB73-291B-47DB-A059-5AADA7C78CBF}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{D22EFB10-AC2A-4D45-9092-206903C33A6C}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{908126EA-7A4C-4101-B145-2DE2E13BC5DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Ajout d'élément dans l'analyse SEO
</commit_message>
<xml_diff>
--- a/P4_01_analyse.xlsx
+++ b/P4_01_analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Formation OC\P4_serra_jahan\jahanSerra_4_03032021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23286C5-F661-45AB-993D-1CC0128BE92C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511C38ED-7786-4E0E-A135-BFBCCB494097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30090" yWindow="3120" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
   <si>
     <t>Catégorie</t>
   </si>
@@ -66,9 +66,6 @@
     <t>utiliser la bonne langue dans la balise en lien avec le site si les textes sont en anglais mettre :en</t>
   </si>
   <si>
-    <t>mettre fr ici</t>
-  </si>
-  <si>
     <t>https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>remplir la meta description avec un texte qui donne envie aux internaute de cliquer</t>
   </si>
   <si>
-    <t>remplir le texte avec un minimum de 70 caractères et un max de 320 caractères</t>
-  </si>
-  <si>
     <t>Acessibilité</t>
   </si>
   <si>
@@ -111,45 +105,27 @@
     <t>bien écrire les liens des pages pour orienter l'utilisateur</t>
   </si>
   <si>
-    <t>remplacer page2&gt; par Contact</t>
-  </si>
-  <si>
     <t>pas de balise sémentique</t>
   </si>
   <si>
     <t>absence de balise comme header main footer et section</t>
   </si>
   <si>
-    <t>utiliser des balises sémentique</t>
-  </si>
-  <si>
-    <t>utiliser des balises section pour compartimenter le site et permettre au robot de scroll plus vite le site et donc de gagner en performance</t>
-  </si>
-  <si>
     <t>href des icones footer redirigent vers index.html</t>
   </si>
   <si>
     <t>mauvais link sur les icones</t>
   </si>
   <si>
-    <t>modifier par les url adéquat selon l'icone exemple page twitter</t>
-  </si>
-  <si>
     <t>pas de balise descriptive sur les images ou mauvaise</t>
   </si>
   <si>
-    <t>associer les bons liens pertinants</t>
-  </si>
-  <si>
     <t>souvent la même balise alt</t>
   </si>
   <si>
     <t>utiliser la balise alt pour décrire l'image afin d'être en cohérence avec la WCAG</t>
   </si>
   <si>
-    <t>modifier les alt selon l'image avec des mots descriptif</t>
-  </si>
-  <si>
     <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6940878-decouvrez-les-exigences-en-matiere-daccessibilite</t>
   </si>
   <si>
@@ -162,9 +138,6 @@
     <t>Optimiser la taille des images</t>
   </si>
   <si>
-    <t>redimensionner les grandes images voir compresser dans la mesure du possible pour gagner au temps de chargement de la page</t>
-  </si>
-  <si>
     <t xml:space="preserve">Changer le titre par un plus cohérent 65 caractères max </t>
   </si>
   <si>
@@ -198,14 +171,119 @@
     <t>Utiliser une encre de retour en haut de page pour l'Accessibilité</t>
   </si>
   <si>
-    <t>création de l'id et de la balise de retour en haut de page</t>
+    <t>Mettre fr ici</t>
+  </si>
+  <si>
+    <t>Remplir le texte avec un minimum de 70 caractères et un max de 320 caractères</t>
+  </si>
+  <si>
+    <t>Remplacer page2&gt; par Contact</t>
+  </si>
+  <si>
+    <t>Utiliser des balises section pour compartimenter le site et permettre au robot de scroll plus Vite le site et donc de gagner en performance</t>
+  </si>
+  <si>
+    <t>Modifier les alt selon l'image avec des mots descriptif</t>
+  </si>
+  <si>
+    <t>Modifier par les url adéquat selon l'icone exemple page twitter</t>
+  </si>
+  <si>
+    <t>Redimensionner les grandes images voir compresser dans la mesure du possible pour gagner au temps de chargement de la page</t>
+  </si>
+  <si>
+    <t>Création de l'id et de la balise de retour en haut de page</t>
+  </si>
+  <si>
+    <t>utiliser des balises sémantique</t>
+  </si>
+  <si>
+    <t>associer les bons liens pertinents</t>
+  </si>
+  <si>
+    <t>Utilisation de couleur trop vive ou non perseptible par une tranche de la population</t>
+  </si>
+  <si>
+    <t>Couleur et contrast trop vif ou trop terne</t>
+  </si>
+  <si>
+    <t>Un contraste dont le ratio est de 4.5:1 pour les textes normaux (dont la fonte est inférieure à 18 points ou 14 points en gras) ;</t>
+  </si>
+  <si>
+    <t>Changer certaines font et association de couleurs : exemple eviter le orange et blanc ensemble</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/WCAG/</t>
+  </si>
+  <si>
+    <t>Absence de l'outils analytics</t>
+  </si>
+  <si>
+    <t>pas de script analytics présent dans le code</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/3013736-comprenez-votre-audience-avec-google-analytics</t>
+  </si>
+  <si>
+    <t>Ajouter le script et lié la propriété sur google analytics</t>
+  </si>
+  <si>
+    <t>Pour améliorer en continu la performance de vos actions Web Marketing, vous allez avoir besoin de collecter, de présenter et d’interpréter des données.</t>
+  </si>
+  <si>
+    <t>Tentative de Backlink abusive</t>
+  </si>
+  <si>
+    <t>Trop de lien externe vers des sources sans lien avec le contenu du site</t>
+  </si>
+  <si>
+    <t>https://www.referenseo.com/blog/liens-externes-booster-referencement/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> prendre des liens dans une thématique proche de la votre</t>
+  </si>
+  <si>
+    <t>Suppression des link dans le footer</t>
+  </si>
+  <si>
+    <t>page2&gt; erreur dans le link des fichiers script</t>
+  </si>
+  <si>
+    <t>la source du script est en .min.js hors dans notre fichier il est en .js simplement</t>
+  </si>
+  <si>
+    <t>Faire un choix soit minifier les fichiers script  pour libérer de l'espace ou alors changer le script par .JS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utiliser les bons script </t>
+  </si>
+  <si>
+    <t>https://www.pierre-giraud.com/bootstrap-apprendre-cours/</t>
+  </si>
+  <si>
+    <t>10 Recommandations</t>
+  </si>
+  <si>
+    <t>image comprenant du texte</t>
+  </si>
+  <si>
+    <t>les images avec du textes ne sont pas adaptées aux lecteurs d'écrans</t>
+  </si>
+  <si>
+    <t>Ne pas utiliser des images pour du texte</t>
+  </si>
+  <si>
+    <t>Suppression de l'image et Ajout d'une balise &lt;p&gt;</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -225,10 +303,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -238,8 +312,25 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +346,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,18 +374,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -508,7 +609,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -538,7 +639,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -560,7 +663,7 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -572,16 +675,16 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
+      <c r="E2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -589,14 +692,14 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -604,39 +707,39 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>14</v>
+      <c r="E4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -644,19 +747,19 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>14</v>
+      <c r="E6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -664,19 +767,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -684,39 +787,39 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>14</v>
+        <v>29</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>41</v>
+      <c r="F9" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -724,19 +827,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -744,67 +847,156 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>41</v>
+      <c r="F12" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="4"/>
+      <c r="A13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="4"/>
+      <c r="A14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="4"/>
+      <c r="A15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1786,8 +1978,13 @@
     <hyperlink ref="F10" r:id="rId9" xr:uid="{2975BB73-291B-47DB-A059-5AADA7C78CBF}"/>
     <hyperlink ref="F11" r:id="rId10" xr:uid="{D22EFB10-AC2A-4D45-9092-206903C33A6C}"/>
     <hyperlink ref="F12" r:id="rId11" xr:uid="{908126EA-7A4C-4101-B145-2DE2E13BC5DA}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{02C8780D-15A4-43AD-8E3F-581FF6AD3AAE}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{F15A1607-4BCB-4832-ACD2-A44A95D695A0}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{D7415A82-9B42-4AB1-AF39-B4037D51982D}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{8792E925-4713-471F-A27D-6E6B94A11527}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{57DFB1BE-DC0E-4F2B-959C-9B0FF3995C8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>